<commit_message>
Correção da validação de orçamento e melhoria do extrator
</commit_message>
<xml_diff>
--- a/output/resultado.xlsx
+++ b/output/resultado.xlsx
@@ -7,17 +7,22 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Relatório" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <definedNames/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Relatório'!$A$1:$G$4</definedName>
+  </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="[$R$-pt-BR] #,##0.00"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+  </numFmts>
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -28,13 +33,22 @@
     <font>
       <b val="1"/>
     </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="004F81BD"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -55,11 +69,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -428,43 +447,53 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="17" customWidth="1" min="1" max="1"/>
+    <col width="9" customWidth="1" min="2" max="2"/>
+    <col width="13" customWidth="1" min="3" max="3"/>
+    <col width="18" customWidth="1" min="4" max="4"/>
+    <col width="17" customWidth="1" min="5" max="5"/>
+    <col width="24" customWidth="1" min="6" max="6"/>
+    <col width="17" customWidth="1" min="7" max="7"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Municipio</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Estado</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Data</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Orcamento</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Prefeito</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>Secretario_Financeiro</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="2" t="inlineStr">
         <is>
           <t>Arquivo</t>
         </is>
@@ -481,13 +510,13 @@
           <t>SP</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="3" t="inlineStr">
         <is>
           <t>15/03/2024</t>
         </is>
       </c>
-      <c r="D2" t="n">
-        <v>12450000</v>
+      <c r="D2" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -516,13 +545,13 @@
           <t>MG</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="3" t="inlineStr">
         <is>
           <t>02/07/2024</t>
         </is>
       </c>
-      <c r="D3" t="n">
-        <v>8980500.75</v>
+      <c r="D3" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -551,13 +580,13 @@
           <t>PR</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" s="3" t="inlineStr">
         <is>
           <t>28/11/2024</t>
         </is>
       </c>
-      <c r="D4" t="n">
-        <v>21300000</v>
+      <c r="D4" s="4" t="n">
+        <v>0</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -576,6 +605,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G4"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>